<commit_message>
daily but curious landed flights.
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0C560F-8908-4F02-B57F-362AC605BB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8245EB32-56D4-44BE-A9E1-4C3A178D18D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -45,19 +45,19 @@
     <t xml:space="preserve">    }</t>
   </si>
   <si>
-    <t xml:space="preserve">    timeCategories: {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   count: 192,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      'Regular arrivals': 163,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      'Night hour arrivals': 23,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      'Shoulder hour flights': 6</t>
+    <t xml:space="preserve">  landed: { count: 111, timeCategories: { 'Regular arrivals': 111 } },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  scheduled: {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    count: 123,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    timeCategories: { 'Night hour arrivals': 117, 'Regular arrivals': 6 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  },</t>
   </si>
 </sst>
 </file>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FD2104-FE63-4627-855F-F59D2062EFC9}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,192 +440,189 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45409</v>
+        <v>45410</v>
       </c>
       <c r="B2">
-        <v>192</v>
+        <v>111</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>163</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45408</v>
+        <v>45409</v>
       </c>
       <c r="B3">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>211</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45407</v>
+        <v>45408</v>
       </c>
       <c r="B4">
-        <v>202</v>
+        <v>243</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>177</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="B5">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>209</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="B6">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="C6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45404</v>
+        <v>45405</v>
       </c>
       <c r="B7">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45403</v>
+        <v>45404</v>
       </c>
       <c r="B8">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45402</v>
+        <v>45403</v>
       </c>
       <c r="B9">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>166</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45401</v>
+        <v>45402</v>
       </c>
       <c r="B10">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C10">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>45400</v>
+        <v>45401</v>
       </c>
       <c r="B11">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>198</v>
-      </c>
-      <c r="J11" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>45399</v>
+        <v>45400</v>
       </c>
       <c r="B12">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="C12">
         <v>20</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="J12" t="s">
         <v>6</v>
@@ -633,304 +630,324 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>45398</v>
+        <v>45399</v>
       </c>
       <c r="B13">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="C13">
         <v>20</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="J13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>45397</v>
+        <v>45398</v>
       </c>
       <c r="B14">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="C14">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="J14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>45396</v>
+        <v>45397</v>
       </c>
       <c r="B15">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="C15">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>198</v>
+      </c>
+      <c r="J15" t="s">
         <v>9</v>
-      </c>
-      <c r="E15">
-        <v>209</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="B16">
-        <v>197</v>
+        <v>236</v>
       </c>
       <c r="C16">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E16">
-        <v>168</v>
+        <v>209</v>
+      </c>
+      <c r="J16" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>45394</v>
+        <v>45395</v>
       </c>
       <c r="B17">
-        <v>244</v>
+        <v>197</v>
       </c>
       <c r="C17">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17">
-        <v>217</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>45393</v>
+        <v>45394</v>
       </c>
       <c r="B18">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="C18">
         <v>19</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E18">
-        <v>196</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>45392</v>
+        <v>45393</v>
       </c>
       <c r="B19">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C19">
         <v>19</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E19">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>45391</v>
+        <v>45392</v>
       </c>
       <c r="B20">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="C20">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E20">
-        <v>189</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>45390</v>
+        <v>45391</v>
       </c>
       <c r="B21">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="C21">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D21">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>45389</v>
+        <v>45390</v>
       </c>
       <c r="B22">
-        <v>172</v>
+        <v>238</v>
       </c>
       <c r="C22">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22">
-        <v>147</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>45388</v>
+        <v>45389</v>
       </c>
       <c r="B23">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="C23">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E23">
-        <v>119</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>45387</v>
+        <v>45388</v>
       </c>
       <c r="B24">
-        <v>220</v>
+        <v>138</v>
       </c>
       <c r="C24">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>193</v>
-      </c>
-      <c r="I24" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>45386</v>
+        <v>45387</v>
       </c>
       <c r="B25">
+        <v>220</v>
+      </c>
+      <c r="C25">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25">
         <v>193</v>
       </c>
-      <c r="C25">
-        <v>12</v>
-      </c>
-      <c r="D25">
+      <c r="I25" t="s">
         <v>5</v>
-      </c>
-      <c r="E25">
-        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>45385</v>
+        <v>45386</v>
       </c>
       <c r="B26">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="C26">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>203</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>45384</v>
+        <v>45385</v>
       </c>
       <c r="B27">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="C27">
         <v>20</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E27">
-        <v>185</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
+        <v>45384</v>
+      </c>
+      <c r="B28">
+        <v>207</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>45383</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>227</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>19</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>4</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <f>SUM(B2:B28)</f>
-        <v>5748</v>
-      </c>
-      <c r="C29">
-        <f t="shared" ref="C29:E29" si="0">SUM(C2:C28)</f>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f>SUM(B2:B29)</f>
+        <v>5859</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:E30" si="0">SUM(C2:C29)</f>
         <v>521</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <f t="shared" si="0"/>
-        <v>5069</v>
+        <v>5180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daily and aviation edge annual data for brs and a few more
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8553DFD6-BB85-47E2-809B-068B764A2118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D92001-F499-4687-9F2A-2BA2E1A1F008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="600" windowWidth="12180" windowHeight="10920" activeTab="1" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,16 +49,16 @@
     <t xml:space="preserve">    timeCategories: {</t>
   </si>
   <si>
-    <t>count: 264,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      'Regular arrivals': 231,</t>
-  </si>
-  <si>
     <t xml:space="preserve">      'Night hour arrivals': 26,</t>
   </si>
   <si>
-    <t xml:space="preserve">      'Shoulder hour flights': 7</t>
+    <t xml:space="preserve">  count: 203,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      'Regular arrivals': 168,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      'Shoulder hour flights': 9</t>
   </si>
 </sst>
 </file>
@@ -953,10 +953,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE8A7C-0A43-4190-8997-8D67F3456349}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,210 +983,227 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45422</v>
+        <v>45423</v>
       </c>
       <c r="B2">
-        <v>264</v>
+        <v>203</v>
       </c>
       <c r="C2">
         <v>26</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>231</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45421</v>
+        <v>45422</v>
       </c>
       <c r="B3">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>214</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45420</v>
+        <v>45421</v>
       </c>
       <c r="B4">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>194</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45419</v>
+        <v>45420</v>
       </c>
       <c r="B5">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C5">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B6">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>217</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45417</v>
+        <v>45418</v>
       </c>
       <c r="B7">
         <v>251</v>
       </c>
       <c r="C7">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>7</v>
       </c>
       <c r="E7">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45416</v>
+        <v>45417</v>
       </c>
       <c r="B8">
-        <v>212</v>
+        <v>251</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>182</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45415</v>
+        <v>45416</v>
       </c>
       <c r="B9">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E9">
-        <v>199</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B10">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="C10">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>188</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>45413</v>
+        <v>45414</v>
       </c>
       <c r="B11">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="C11">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45413</v>
+      </c>
+      <c r="B12">
+        <v>229</v>
+      </c>
+      <c r="C12">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
         <v>202</v>
       </c>
-      <c r="H11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <f>SUM(B2:B11)</f>
-        <v>2335</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ref="C12:E12" si="0">SUM(C2:C11)</f>
-        <v>232</v>
-      </c>
-      <c r="D12">
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>SUM(B2:B12)</f>
+        <v>2538</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:E13" si="0">SUM(C2:C12)</f>
+        <v>258</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="E12">
+        <v>64</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="0"/>
-        <v>2048</v>
-      </c>
-      <c r="H12" t="s">
+        <v>2216</v>
+      </c>
+      <c r="H13" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H13" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
18 and 19 May
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C162065-B812-4E7A-883C-203FEA2C3757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE486A-0279-486A-9F1A-805CBEBA8BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>date</t>
   </si>
@@ -44,21 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">    }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    timeCategories: {</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> count: 224,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      'Regular arrivals': 199,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      'Night hour arrivals': 18,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      'Shoulder hour flights': 7</t>
   </si>
 </sst>
 </file>
@@ -953,10 +938,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE8A7C-0A43-4190-8997-8D67F3456349}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +949,7 @@
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -981,279 +966,264 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45429</v>
+        <v>45431</v>
       </c>
       <c r="B2">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45428</v>
+        <v>45430</v>
       </c>
       <c r="B3">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="C3">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45427</v>
+        <v>45429</v>
       </c>
       <c r="B4">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="B5">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="C5">
         <v>28</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45425</v>
+        <v>45427</v>
       </c>
       <c r="B6">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="C6">
         <v>27</v>
       </c>
       <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45426</v>
+      </c>
+      <c r="B7">
+        <v>231</v>
+      </c>
+      <c r="C7">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B8">
+        <v>227</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>45424</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>242</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>23</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>45423</v>
-      </c>
-      <c r="B8">
-        <v>203</v>
-      </c>
-      <c r="C8">
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>45422</v>
-      </c>
-      <c r="B9">
-        <v>264</v>
-      </c>
-      <c r="C9">
-        <v>26</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45423</v>
+      </c>
+      <c r="B10">
+        <v>203</v>
+      </c>
+      <c r="C10">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45422</v>
+      </c>
+      <c r="B11">
+        <v>264</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>45421</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>247</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>25</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>8</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>45420</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>223</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>24</v>
       </c>
-      <c r="D11">
+      <c r="D13">
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="E13">
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>45419</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>227</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <v>26</v>
       </c>
-      <c r="D12">
+      <c r="D14">
         <v>6</v>
       </c>
-      <c r="E12">
+      <c r="E14">
         <v>195</v>
       </c>
-      <c r="I12" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45418</v>
+      </c>
+      <c r="B15">
+        <v>251</v>
+      </c>
+      <c r="C15">
+        <v>27</v>
+      </c>
+      <c r="D15">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>45418</v>
-      </c>
-      <c r="B13">
+      <c r="E15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45417</v>
+      </c>
+      <c r="B16">
         <v>251</v>
       </c>
-      <c r="C13">
-        <v>27</v>
-      </c>
-      <c r="D13">
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16">
         <v>7</v>
       </c>
-      <c r="E13">
-        <v>217</v>
-      </c>
-      <c r="I13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>45417</v>
-      </c>
-      <c r="B14">
-        <v>251</v>
-      </c>
-      <c r="C14">
-        <v>18</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-      <c r="E14">
+      <c r="E16">
         <v>226</v>
-      </c>
-      <c r="I14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>45416</v>
-      </c>
-      <c r="B15">
-        <v>212</v>
-      </c>
-      <c r="C15">
-        <v>21</v>
-      </c>
-      <c r="D15">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>182</v>
-      </c>
-      <c r="I15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>45415</v>
-      </c>
-      <c r="B16">
-        <v>219</v>
-      </c>
-      <c r="C16">
-        <v>20</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>199</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>45414</v>
+        <v>45416</v>
       </c>
       <c r="B17">
         <v>212</v>
@@ -1262,45 +1232,79 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E17">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
+        <v>45415</v>
+      </c>
+      <c r="B18">
+        <v>219</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45414</v>
+      </c>
+      <c r="B19">
+        <v>212</v>
+      </c>
+      <c r="C19">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>45413</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>229</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <v>24</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>3</v>
       </c>
-      <c r="E18">
+      <c r="E20">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <f>SUM(B2:B18)</f>
-        <v>3955</v>
-      </c>
-      <c r="C19">
-        <f t="shared" ref="C19:E19" si="0">SUM(C2:C18)</f>
-        <v>409</v>
-      </c>
-      <c r="D19">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f>SUM(B2:B20)</f>
+        <v>4408</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:E21" si="0">SUM(C2:C20)</f>
+        <v>452</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="E19">
+        <v>108</v>
+      </c>
+      <c r="E21">
         <f t="shared" si="0"/>
-        <v>3450</v>
+        <v>3848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daily 20 and 21 may
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE486A-0279-486A-9F1A-805CBEBA8BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73188C3-1D0D-4DE9-B44A-1D111EBAEB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -938,10 +938,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE8A7C-0A43-4190-8997-8D67F3456349}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,296 +968,296 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45431</v>
+        <v>45433</v>
       </c>
       <c r="B2">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45430</v>
+        <v>45432</v>
       </c>
       <c r="B3">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3">
-        <v>187</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45429</v>
+        <v>45431</v>
       </c>
       <c r="B4">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="C4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45428</v>
+        <v>45430</v>
       </c>
       <c r="B5">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="C5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>211</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45427</v>
+        <v>45429</v>
       </c>
       <c r="B6">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="B7">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="C7">
         <v>28</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45425</v>
+        <v>45427</v>
       </c>
       <c r="B8">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="C8">
         <v>27</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>198</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45424</v>
+        <v>45426</v>
       </c>
       <c r="B9">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C9">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45423</v>
+        <v>45425</v>
       </c>
       <c r="B10">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>168</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>45422</v>
+        <v>45424</v>
       </c>
       <c r="B11">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="C11">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>7</v>
       </c>
       <c r="E11">
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>45421</v>
+        <v>45423</v>
       </c>
       <c r="B12">
-        <v>247</v>
+        <v>203</v>
       </c>
       <c r="C12">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12">
-        <v>214</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>45420</v>
+        <v>45422</v>
       </c>
       <c r="B13">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="C13">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E13">
-        <v>194</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B14">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="C14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E14">
-        <v>195</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>45418</v>
+        <v>45420</v>
       </c>
       <c r="B15">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C15">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>217</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>45417</v>
+        <v>45419</v>
       </c>
       <c r="B16">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C16">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>226</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>45416</v>
+        <v>45418</v>
       </c>
       <c r="B17">
-        <v>212</v>
+        <v>251</v>
       </c>
       <c r="C17">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E17">
-        <v>182</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>45415</v>
+        <v>45417</v>
       </c>
       <c r="B18">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="C18">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>199</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>45414</v>
+        <v>45416</v>
       </c>
       <c r="B19">
         <v>212</v>
@@ -1266,45 +1266,79 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
+        <v>45415</v>
+      </c>
+      <c r="B20">
+        <v>219</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45414</v>
+      </c>
+      <c r="B21">
+        <v>212</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>45413</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>229</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <v>24</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <v>3</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f>SUM(B2:B20)</f>
-        <v>4408</v>
-      </c>
-      <c r="C21">
-        <f t="shared" ref="C21:E21" si="0">SUM(C2:C20)</f>
-        <v>452</v>
-      </c>
-      <c r="D21">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f>SUM(B2:B22)</f>
+        <v>4870</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:E23" si="0">SUM(C2:C22)</f>
+        <v>501</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="E21">
+        <v>114</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="0"/>
-        <v>3848</v>
+        <v>4255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daily 22 and 23 may
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73188C3-1D0D-4DE9-B44A-1D111EBAEB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A06934-BF92-4AF8-A84D-1BEC282F6BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -44,6 +44,21 @@
   </si>
   <si>
     <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    timeCategories: {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      'Regular arrivals': 210,</t>
+  </si>
+  <si>
+    <t>count: 243,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      'Night hour arrivals': 26,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      'Shoulder hour flights': 7</t>
   </si>
 </sst>
 </file>
@@ -938,10 +953,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE8A7C-0A43-4190-8997-8D67F3456349}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,7 +964,7 @@
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -966,332 +981,347 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45433</v>
+        <v>45435</v>
       </c>
       <c r="B2">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45432</v>
+        <v>45434</v>
       </c>
       <c r="B3">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="C3">
         <v>24</v>
       </c>
       <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45433</v>
+      </c>
+      <c r="B4">
+        <v>230</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>45431</v>
-      </c>
-      <c r="B4">
-        <v>240</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
       <c r="E4">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45430</v>
+        <v>45432</v>
       </c>
       <c r="B5">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45429</v>
+        <v>45431</v>
       </c>
       <c r="B6">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="C6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E6">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45428</v>
+        <v>45430</v>
       </c>
       <c r="B7">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="C7">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45427</v>
+        <v>45429</v>
       </c>
       <c r="B8">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="B9">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="C9">
         <v>28</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45425</v>
+        <v>45427</v>
       </c>
       <c r="B10">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="C10">
         <v>27</v>
       </c>
       <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>219</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45426</v>
+      </c>
+      <c r="B11">
+        <v>231</v>
+      </c>
+      <c r="C11">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>195</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45425</v>
+      </c>
+      <c r="B12">
+        <v>227</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>198</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>45424</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>242</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>23</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-      <c r="E11">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>45423</v>
-      </c>
-      <c r="B12">
-        <v>203</v>
-      </c>
-      <c r="C12">
-        <v>26</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>45422</v>
-      </c>
-      <c r="B13">
-        <v>264</v>
-      </c>
-      <c r="C13">
-        <v>26</v>
       </c>
       <c r="D13">
         <v>7</v>
       </c>
       <c r="E13">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45423</v>
+      </c>
+      <c r="B14">
+        <v>203</v>
+      </c>
+      <c r="C14">
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45422</v>
+      </c>
+      <c r="B15">
+        <v>264</v>
+      </c>
+      <c r="C15">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>45421</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>247</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>25</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <v>8</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>45420</v>
-      </c>
-      <c r="B15">
-        <v>223</v>
-      </c>
-      <c r="C15">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>45419</v>
-      </c>
-      <c r="B16">
-        <v>227</v>
-      </c>
-      <c r="C16">
-        <v>26</v>
-      </c>
-      <c r="D16">
-        <v>6</v>
-      </c>
-      <c r="E16">
-        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>45418</v>
+        <v>45420</v>
       </c>
       <c r="B17">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C17">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>217</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>45417</v>
+        <v>45419</v>
       </c>
       <c r="B18">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C18">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>226</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>45416</v>
+        <v>45418</v>
       </c>
       <c r="B19">
-        <v>212</v>
+        <v>251</v>
       </c>
       <c r="C19">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19">
-        <v>182</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>45415</v>
+        <v>45417</v>
       </c>
       <c r="B20">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>199</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>45414</v>
+        <v>45416</v>
       </c>
       <c r="B21">
         <v>212</v>
@@ -1300,45 +1330,79 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E21">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
+        <v>45415</v>
+      </c>
+      <c r="B22">
+        <v>219</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45414</v>
+      </c>
+      <c r="B23">
+        <v>212</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>45413</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>229</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>24</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>3</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <f>SUM(B2:B22)</f>
-        <v>4870</v>
-      </c>
-      <c r="C23">
-        <f t="shared" ref="C23:E23" si="0">SUM(C2:C22)</f>
-        <v>501</v>
-      </c>
-      <c r="D23">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f>SUM(B2:B24)</f>
+        <v>5355</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:E25" si="0">SUM(C2:C24)</f>
+        <v>551</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="0"/>
-        <v>114</v>
-      </c>
-      <c r="E23">
+        <v>129</v>
+      </c>
+      <c r="E25">
         <f t="shared" si="0"/>
-        <v>4255</v>
+        <v>4675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daily 28 and 29 May
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E33EBF-4501-43F1-9375-AA2B6944B425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348FDA34-E784-47F7-8901-2FDD980BB7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -49,16 +49,16 @@
     <t xml:space="preserve">    timeCategories: {</t>
   </si>
   <si>
-    <t>count: 214,</t>
+    <t>count: 252,</t>
   </si>
   <si>
-    <t xml:space="preserve">      'Regular arrivals': 187,</t>
+    <t xml:space="preserve">      'Regular arrivals': 222,</t>
   </si>
   <si>
-    <t xml:space="preserve">      'Night hour arrivals': 21,</t>
+    <t xml:space="preserve">      'Night hour arrivals': 26,</t>
   </si>
   <si>
-    <t xml:space="preserve">      'Shoulder hour flights': 6</t>
+    <t xml:space="preserve">      'Shoulder hour flights': 4</t>
   </si>
 </sst>
 </file>
@@ -953,10 +953,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE8A7C-0A43-4190-8997-8D67F3456349}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,447 +983,447 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45439</v>
+        <v>45441</v>
       </c>
       <c r="B2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45438</v>
+        <v>45440</v>
       </c>
       <c r="B3">
-        <v>186</v>
+        <v>247</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>162</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45437</v>
+        <v>45439</v>
       </c>
       <c r="B4">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>187</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45436</v>
+        <v>45438</v>
       </c>
       <c r="B5">
-        <v>248</v>
+        <v>186</v>
       </c>
       <c r="C5">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>212</v>
+        <v>162</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45435</v>
+        <v>45437</v>
       </c>
       <c r="B6">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="C6">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>210</v>
+        <v>187</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45434</v>
+        <v>45436</v>
       </c>
       <c r="B7">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C7">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>212</v>
+      </c>
+      <c r="H7" t="s">
         <v>8</v>
-      </c>
-      <c r="E7">
-        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45433</v>
+        <v>45435</v>
       </c>
       <c r="B8">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="C8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="H8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45432</v>
+        <v>45434</v>
       </c>
       <c r="B9">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="C9">
         <v>24</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="H9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45431</v>
+        <v>45433</v>
       </c>
       <c r="B10">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>211</v>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>45430</v>
+        <v>45432</v>
       </c>
       <c r="B11">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C11">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11">
-        <v>187</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>45429</v>
+        <v>45431</v>
       </c>
       <c r="B12">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="C12">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E12">
-        <v>199</v>
-      </c>
-      <c r="H12" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>45428</v>
+        <v>45430</v>
       </c>
       <c r="B13">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="C13">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13">
-        <v>211</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>45427</v>
+        <v>45429</v>
       </c>
       <c r="B14">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="C14">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="B15">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="C15">
         <v>28</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>45425</v>
+        <v>45427</v>
       </c>
       <c r="B16">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="C16">
         <v>27</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>198</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>45424</v>
+        <v>45426</v>
       </c>
       <c r="B17">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C17">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E17">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>45423</v>
+        <v>45425</v>
       </c>
       <c r="B18">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C18">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D18">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>168</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>45422</v>
+        <v>45424</v>
       </c>
       <c r="B19">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="C19">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19">
         <v>7</v>
       </c>
       <c r="E19">
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>45421</v>
+        <v>45423</v>
       </c>
       <c r="B20">
-        <v>247</v>
+        <v>203</v>
       </c>
       <c r="C20">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E20">
-        <v>214</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>45420</v>
+        <v>45422</v>
       </c>
       <c r="B21">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="C21">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E21">
-        <v>194</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B22">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="C22">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E22">
-        <v>195</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>45418</v>
+        <v>45420</v>
       </c>
       <c r="B23">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C23">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E23">
-        <v>217</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>45417</v>
+        <v>45419</v>
       </c>
       <c r="B24">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C24">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>226</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>45416</v>
+        <v>45418</v>
       </c>
       <c r="B25">
-        <v>212</v>
+        <v>251</v>
       </c>
       <c r="C25">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E25">
-        <v>182</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>45415</v>
+        <v>45417</v>
       </c>
       <c r="B26">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="C26">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E26">
-        <v>199</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>45414</v>
+        <v>45416</v>
       </c>
       <c r="B27">
         <v>212</v>
@@ -1432,45 +1432,79 @@
         <v>21</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E27">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
+        <v>45415</v>
+      </c>
+      <c r="B28">
+        <v>219</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45414</v>
+      </c>
+      <c r="B29">
+        <v>212</v>
+      </c>
+      <c r="C29">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>45413</v>
       </c>
-      <c r="B28">
+      <c r="B30">
         <v>229</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>24</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>3</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <f>SUM(B2:B28)</f>
-        <v>6256</v>
-      </c>
-      <c r="C29">
-        <f t="shared" ref="C29:E29" si="0">SUM(C2:C28)</f>
-        <v>660</v>
-      </c>
-      <c r="D29">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f>SUM(B2:B30)</f>
+        <v>6755</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:E31" si="0">SUM(C2:C30)</f>
+        <v>715</v>
+      </c>
+      <c r="D31">
         <f t="shared" si="0"/>
-        <v>143</v>
-      </c>
-      <c r="E29">
+        <v>152</v>
+      </c>
+      <c r="E31">
         <f t="shared" si="0"/>
-        <v>5453</v>
+        <v>5888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
30, 31 may and 1 June
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348FDA34-E784-47F7-8901-2FDD980BB7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607CCBE6-C3A0-44FD-8A2E-7B1FF44E2DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="May" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -49,16 +50,28 @@
     <t xml:space="preserve">    timeCategories: {</t>
   </si>
   <si>
-    <t>count: 252,</t>
+    <t xml:space="preserve">  count: 267,</t>
   </si>
   <si>
-    <t xml:space="preserve">      'Regular arrivals': 222,</t>
+    <t xml:space="preserve">      'Regular arrivals': 236,</t>
   </si>
   <si>
-    <t xml:space="preserve">      'Night hour arrivals': 26,</t>
+    <t xml:space="preserve">      'Shoulder hour flights': 7,</t>
   </si>
   <si>
-    <t xml:space="preserve">      'Shoulder hour flights': 4</t>
+    <t xml:space="preserve">      'Night hour arrivals': 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> count: 209,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      'Regular arrivals': 173,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      'Night hour arrivals': 30,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      'Shoulder hour flights': 6</t>
   </si>
 </sst>
 </file>
@@ -953,10 +966,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE8A7C-0A43-4190-8997-8D67F3456349}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,481 +996,481 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45441</v>
+        <v>45443</v>
       </c>
       <c r="B2">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="C2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E2">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45440</v>
+        <v>45442</v>
       </c>
       <c r="B3">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C3">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45439</v>
+        <v>45441</v>
       </c>
       <c r="B4">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C4">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45438</v>
+        <v>45440</v>
       </c>
       <c r="B5">
-        <v>186</v>
+        <v>247</v>
       </c>
       <c r="C5">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>162</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45437</v>
+        <v>45439</v>
       </c>
       <c r="B6">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="C6">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>187</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45436</v>
+        <v>45438</v>
       </c>
       <c r="B7">
-        <v>248</v>
+        <v>186</v>
       </c>
       <c r="C7">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>212</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45435</v>
+        <v>45437</v>
       </c>
       <c r="B8">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="C8">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>210</v>
-      </c>
-      <c r="H8" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45434</v>
+        <v>45436</v>
       </c>
       <c r="B9">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C9">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>210</v>
-      </c>
-      <c r="H9" t="s">
-        <v>10</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45433</v>
+        <v>45435</v>
       </c>
       <c r="B10">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>202</v>
+        <v>210</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>45432</v>
+        <v>45434</v>
       </c>
       <c r="B11">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="C11">
         <v>24</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>205</v>
+        <v>210</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>45431</v>
+        <v>45433</v>
       </c>
       <c r="B12">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>211</v>
+        <v>202</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>45430</v>
+        <v>45432</v>
       </c>
       <c r="B13">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C13">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13">
-        <v>187</v>
+        <v>205</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>45429</v>
+        <v>45431</v>
       </c>
       <c r="B14">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="C14">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E14">
-        <v>199</v>
+        <v>211</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>45428</v>
+        <v>45430</v>
       </c>
       <c r="B15">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="C15">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="E15">
-        <v>211</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>45427</v>
+        <v>45429</v>
       </c>
       <c r="B16">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="C16">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E16">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="B17">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="C17">
         <v>28</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>45425</v>
+        <v>45427</v>
       </c>
       <c r="B18">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="C18">
         <v>27</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>198</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>45424</v>
+        <v>45426</v>
       </c>
       <c r="B19">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C19">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>45423</v>
+        <v>45425</v>
       </c>
       <c r="B20">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>168</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>45422</v>
+        <v>45424</v>
       </c>
       <c r="B21">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="C21">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D21">
         <v>7</v>
       </c>
       <c r="E21">
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>45421</v>
+        <v>45423</v>
       </c>
       <c r="B22">
-        <v>247</v>
+        <v>203</v>
       </c>
       <c r="C22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22">
-        <v>214</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>45420</v>
+        <v>45422</v>
       </c>
       <c r="B23">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="C23">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>194</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B24">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="C24">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E24">
-        <v>195</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>45418</v>
+        <v>45420</v>
       </c>
       <c r="B25">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C25">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>217</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>45417</v>
+        <v>45419</v>
       </c>
       <c r="B26">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C26">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26">
-        <v>226</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>45416</v>
+        <v>45418</v>
       </c>
       <c r="B27">
-        <v>212</v>
+        <v>251</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E27">
-        <v>182</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>45415</v>
+        <v>45417</v>
       </c>
       <c r="B28">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="C28">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>199</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>45414</v>
+        <v>45416</v>
       </c>
       <c r="B29">
         <v>212</v>
@@ -1466,45 +1479,156 @@
         <v>21</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E29">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
+        <v>45415</v>
+      </c>
+      <c r="B30">
+        <v>219</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>45414</v>
+      </c>
+      <c r="B31">
+        <v>212</v>
+      </c>
+      <c r="C31">
+        <v>21</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>45413</v>
       </c>
-      <c r="B30">
+      <c r="B32">
         <v>229</v>
       </c>
-      <c r="C30">
+      <c r="C32">
         <v>24</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <v>3</v>
       </c>
-      <c r="E30">
+      <c r="E32">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <f>SUM(B2:B30)</f>
-        <v>6755</v>
-      </c>
-      <c r="C31">
-        <f t="shared" ref="C31:E31" si="0">SUM(C2:C30)</f>
-        <v>715</v>
-      </c>
-      <c r="D31">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f>SUM(B2:B32)</f>
+        <v>7270</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:E33" si="0">SUM(C2:C32)</f>
+        <v>767</v>
+      </c>
+      <c r="D33">
         <f t="shared" si="0"/>
-        <v>152</v>
-      </c>
-      <c r="E31">
+        <v>167</v>
+      </c>
+      <c r="E33">
         <f t="shared" si="0"/>
-        <v>5888</v>
+        <v>6336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A5490-12E2-4F9B-9F0D-8B54A0D55008}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45444</v>
+      </c>
+      <c r="B2">
+        <v>209</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated LBA data and daily for BRS
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A7AF79-C3ED-4A17-9B05-4ECDEC353CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB42054F-6945-4999-8F65-67AC6214EF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -1549,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A5490-12E2-4F9B-9F0D-8B54A0D55008}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:H13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,54 +1579,71 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45445</v>
+        <v>45446</v>
       </c>
       <c r="B2">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="C2">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
+        <v>45445</v>
+      </c>
+      <c r="B3">
+        <v>252</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>45444</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>209</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>30</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>6</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>SUM(B2:B3)</f>
-        <v>461</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:E4" si="0">SUM(C2:C3)</f>
-        <v>56</v>
-      </c>
-      <c r="D4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>SUM(B2:B4)</f>
+        <v>673</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C2:C4)</f>
+        <v>57</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daily with some missing data
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB42054F-6945-4999-8F65-67AC6214EF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34862481-AE84-4B1E-BDFF-C5AEE74C35DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -1549,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A5490-12E2-4F9B-9F0D-8B54A0D55008}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,10 +1579,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45446</v>
+        <v>45449</v>
       </c>
       <c r="B2">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1591,59 +1591,110 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45445</v>
+        <v>45448</v>
       </c>
       <c r="B3">
-        <v>252</v>
+        <v>141</v>
       </c>
       <c r="C3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>217</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
+        <v>45447</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45446</v>
+      </c>
+      <c r="B5">
+        <v>212</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45445</v>
+      </c>
+      <c r="B6">
+        <v>252</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>45444</v>
       </c>
-      <c r="B4">
+      <c r="B7">
         <v>209</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <v>30</v>
       </c>
-      <c r="D4">
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="E7">
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <f>SUM(B2:B4)</f>
-        <v>673</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="C5:E5" si="0">SUM(C2:C4)</f>
-        <v>57</v>
-      </c>
-      <c r="D5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>815</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="0">SUM(C2:C7)</f>
+        <v>85</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E5">
+        <v>18</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>601</v>
+        <v>712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update from 11 to 14 June
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C05B9A5-F9F0-4490-B52F-E2E068B86CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE76AFA-9ED4-47CA-82A1-AD3666F0A6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="0" windowWidth="12180" windowHeight="10920" activeTab="3" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
   <sheets>
     <sheet name="April" sheetId="1" r:id="rId1"/>
@@ -1556,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A5490-12E2-4F9B-9F0D-8B54A0D55008}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,7 +1567,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1584,156 +1584,223 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
+        <v>45457</v>
+      </c>
+      <c r="B2">
+        <v>242</v>
+      </c>
+      <c r="C2">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45456</v>
+      </c>
+      <c r="B3">
+        <v>246</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45455</v>
+      </c>
+      <c r="B4">
+        <v>251</v>
+      </c>
+      <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>45454</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="B5">
+        <v>242</v>
+      </c>
+      <c r="C5">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>45453</v>
       </c>
-      <c r="B3">
+      <c r="B6">
         <v>174</v>
       </c>
-      <c r="C3">
+      <c r="C6">
         <v>28</v>
       </c>
-      <c r="D3">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="E6">
+        <v>145</v>
+      </c>
+      <c r="J6">
+        <f>222+(C2+C3+C4+C5)</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>45452</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>45451</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>45450</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>45449</v>
       </c>
-      <c r="B7">
+      <c r="B10">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>45448</v>
-      </c>
-      <c r="B8">
-        <v>141</v>
-      </c>
-      <c r="C8">
-        <v>27</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>45447</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>45446</v>
-      </c>
-      <c r="B10">
-        <v>212</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45448</v>
+      </c>
+      <c r="B11">
+        <v>141</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45447</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45446</v>
+      </c>
+      <c r="B13">
+        <v>212</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>45445</v>
       </c>
-      <c r="B11">
+      <c r="B14">
         <v>252</v>
       </c>
-      <c r="C11">
+      <c r="C14">
         <v>26</v>
       </c>
-      <c r="D11">
+      <c r="D14">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="E14">
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>45444</v>
       </c>
-      <c r="B12">
+      <c r="B15">
         <v>209</v>
       </c>
-      <c r="C12">
+      <c r="C15">
         <v>30</v>
       </c>
-      <c r="D12">
+      <c r="D15">
         <v>6</v>
       </c>
-      <c r="E12">
+      <c r="E15">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16">
         <v>988</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <v>112</v>
       </c>
-      <c r="D13">
+      <c r="D16">
         <v>19</v>
       </c>
-      <c r="E13">
+      <c r="E16">
         <v>757</v>
       </c>
     </row>
@@ -1746,7 +1813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747F78A1-D843-4C0C-8CEA-32B089F68384}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E72" sqref="A1:E72"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
daily and last year data
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE76AFA-9ED4-47CA-82A1-AD3666F0A6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D4E23A-14C2-4E42-8EC0-A3945AAFB42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -1556,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A5490-12E2-4F9B-9F0D-8B54A0D55008}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,7 +1567,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1584,223 +1584,307 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45457</v>
+        <v>45460</v>
       </c>
       <c r="B2">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="C2">
         <v>26</v>
       </c>
       <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45459</v>
+      </c>
+      <c r="B3">
+        <v>260</v>
+      </c>
+      <c r="C3">
+        <v>27</v>
+      </c>
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="E2">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>45456</v>
-      </c>
-      <c r="B3">
-        <v>246</v>
-      </c>
-      <c r="C3">
-        <v>31</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
       <c r="E3">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45455</v>
+        <v>45458</v>
       </c>
       <c r="B4">
-        <v>251</v>
+        <v>221</v>
       </c>
       <c r="C4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45454</v>
+        <v>45457</v>
       </c>
       <c r="B5">
         <v>242</v>
       </c>
       <c r="C5">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45456</v>
+      </c>
+      <c r="B6">
+        <v>246</v>
+      </c>
+      <c r="C6">
         <v>31</v>
       </c>
-      <c r="D5">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>210</v>
+      </c>
+      <c r="J6">
+        <f>SUM(B2,B3,B4)</f>
+        <v>740</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:M6" si="0">SUM(C2,C3,C4)</f>
+        <v>81</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>642</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45455</v>
+      </c>
+      <c r="B7">
+        <v>251</v>
+      </c>
+      <c r="C7">
+        <v>26</v>
+      </c>
+      <c r="D7">
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="E7">
+        <v>218</v>
+      </c>
+      <c r="J7">
+        <v>3079</v>
+      </c>
+      <c r="K7">
+        <v>336</v>
+      </c>
+      <c r="L7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45454</v>
+      </c>
+      <c r="B8">
+        <v>242</v>
+      </c>
+      <c r="C8">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
         <v>204</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="J8">
+        <f>SUM(J7,J6)</f>
+        <v>3819</v>
+      </c>
+      <c r="K8">
+        <f>SUM(K7,K6)</f>
+        <v>417</v>
+      </c>
+      <c r="L8">
+        <f>SUM(L7,L6)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>45453</v>
       </c>
-      <c r="B6">
+      <c r="B9">
         <v>174</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>28</v>
       </c>
-      <c r="D6">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="E9">
         <v>145</v>
       </c>
-      <c r="J6">
-        <f>222+(C2+C3+C4+C5)</f>
-        <v>336</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>45452</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>45451</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>45450</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>45449</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C13">
         <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>45448</v>
-      </c>
-      <c r="B11">
-        <v>141</v>
-      </c>
-      <c r="C11">
-        <v>27</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>45447</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>45446</v>
-      </c>
-      <c r="B13">
-        <v>212</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45448</v>
+      </c>
+      <c r="B14">
+        <v>141</v>
+      </c>
+      <c r="C14">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45447</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45446</v>
+      </c>
+      <c r="B16">
+        <v>212</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>45445</v>
       </c>
-      <c r="B14">
+      <c r="B17">
         <v>252</v>
       </c>
-      <c r="C14">
+      <c r="C17">
         <v>26</v>
       </c>
-      <c r="D14">
+      <c r="D17">
         <v>9</v>
       </c>
-      <c r="E14">
+      <c r="E17">
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>45444</v>
       </c>
-      <c r="B15">
+      <c r="B18">
         <v>209</v>
       </c>
-      <c r="C15">
+      <c r="C18">
         <v>30</v>
       </c>
-      <c r="D15">
+      <c r="D18">
         <v>6</v>
       </c>
-      <c r="E15">
+      <c r="E18">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19">
         <v>988</v>
       </c>
-      <c r="C16">
+      <c r="C19">
         <v>112</v>
       </c>
-      <c r="D16">
+      <c r="D19">
         <v>19</v>
       </c>
-      <c r="E16">
+      <c r="E19">
         <v>757</v>
       </c>
     </row>

</xml_diff>

<commit_message>
up to july 3
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B332B619-DCF2-4000-895E-846B75E1954B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C791B8D2-F688-4967-A0BB-ECD0BB1770C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
   <sheets>
     <sheet name="April" sheetId="1" r:id="rId1"/>
     <sheet name="May" sheetId="2" r:id="rId2"/>
     <sheet name="June" sheetId="3" r:id="rId3"/>
-    <sheet name="all" sheetId="4" r:id="rId4"/>
+    <sheet name="July" sheetId="5" r:id="rId4"/>
+    <sheet name="all" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>date</t>
   </si>
@@ -1558,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A5490-12E2-4F9B-9F0D-8B54A0D55008}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17:L23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,6 +2181,171 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8506D388-4002-4CB9-8696-E40E6FE36088}">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45474</v>
+      </c>
+      <c r="B2">
+        <v>222</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45475</v>
+      </c>
+      <c r="B3">
+        <v>162</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45476</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45478</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45479</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45480</v>
+      </c>
+      <c r="I8">
+        <f>SUM(B2,B3)</f>
+        <v>384</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:K8" si="0">SUM(C2,C3)</f>
+        <v>41</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45481</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45482</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45485</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45486</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45488</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45489</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45490</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747F78A1-D843-4C0C-8CEA-32B089F68384}">
   <dimension ref="A1:E72"/>
   <sheetViews>

</xml_diff>

<commit_message>
up to July 8
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA12BED-904D-4E5D-8241-7B9E95E5F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE89C03-258F-40D4-A82F-24EE2CD64B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -2185,7 +2185,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,21 +2338,33 @@
         <v>219</v>
       </c>
       <c r="I8">
-        <f>SUM(B2,B3:B8)</f>
-        <v>1611</v>
+        <f>SUM(B2,B3:B9)</f>
+        <v>1883</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:K8" si="0">SUM(C2,C3:C8)</f>
-        <v>211</v>
+        <f t="shared" ref="J8:K8" si="0">SUM(C2,C3:C9)</f>
+        <v>244</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45481</v>
+      </c>
+      <c r="B9">
+        <v>272</v>
+      </c>
+      <c r="C9">
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updat 19 july and also moved files
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37547B2-C062-46D7-95DB-72F671DC2BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52421B8-DA38-4F3A-A152-E57C96B1557D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -2182,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8506D388-4002-4CB9-8696-E40E6FE36088}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="M11" sqref="M11:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,16 +2338,16 @@
         <v>219</v>
       </c>
       <c r="I8">
-        <f>SUM(B2,B3:B19)</f>
-        <v>4395</v>
+        <f>SUM(B2,B3:B20)</f>
+        <v>4588</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:K8" si="0">SUM(C2,C3:C19)</f>
-        <v>584</v>
+        <f t="shared" ref="J8:K8" si="0">SUM(C2,C3:C20)</f>
+        <v>615</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2535,6 +2535,23 @@
       </c>
       <c r="E19">
         <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45492</v>
+      </c>
+      <c r="B20">
+        <v>193</v>
+      </c>
+      <c r="C20">
+        <v>31</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daily up to 29/7
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2583EF7C-E00B-4B36-8804-AAB1A4E372CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF28286-2149-44E5-87E9-677228B5AE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -2182,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8506D388-4002-4CB9-8696-E40E6FE36088}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,16 +2338,16 @@
         <v>219</v>
       </c>
       <c r="I8">
-        <f>SUM(B2,B3:B27)</f>
-        <v>6313</v>
+        <f>SUM(B2,B3:B30)</f>
+        <v>7100</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:K8" si="0">SUM(C2,C3:C27)</f>
-        <v>835</v>
+        <f t="shared" ref="J8:K8" si="0">SUM(C2,C3:C30)</f>
+        <v>935</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>143</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2671,6 +2671,57 @@
       </c>
       <c r="E27">
         <v>223</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45500</v>
+      </c>
+      <c r="B28">
+        <v>232</v>
+      </c>
+      <c r="C28">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45501</v>
+      </c>
+      <c r="B29">
+        <v>278</v>
+      </c>
+      <c r="C29">
+        <v>32</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45502</v>
+      </c>
+      <c r="B30">
+        <v>277</v>
+      </c>
+      <c r="C30">
+        <v>35</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daily plus LL flights
</commit_message>
<xml_diff>
--- a/Daily data_240424a.xlsx
+++ b/Daily data_240424a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josti\OneDrive\Desktop\Gitlab clone\LDR\FlightViz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F852E1-5B11-4894-9A7B-8E1639051C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40980FC5-FE07-4B3C-8381-390643E81270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{40B04361-33FA-49C5-9A9E-2D7704FB1280}"/>
   </bookViews>
@@ -3353,7 +3353,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24:K29"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3507,15 +3507,15 @@
       </c>
       <c r="I8">
         <f>SUM(B2,B3:B32)</f>
-        <v>5593</v>
+        <v>6358</v>
       </c>
       <c r="J8">
         <f>SUM(C2,C3:C32)</f>
-        <v>797</v>
+        <v>900</v>
       </c>
       <c r="K8">
         <f t="shared" ref="K8" si="0">SUM(D2,D3:D32)</f>
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3794,15 +3794,51 @@
       <c r="A25" s="1">
         <v>45559</v>
       </c>
+      <c r="B25">
+        <v>266</v>
+      </c>
+      <c r="C25">
+        <v>41</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>224</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45560</v>
       </c>
+      <c r="B26">
+        <v>262</v>
+      </c>
+      <c r="C26">
+        <v>36</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>219</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45561</v>
+      </c>
+      <c r="B27">
+        <v>237</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>